<commit_message>
wrote about 4.4.7-8 and rearanged so all the answers are in the same folder
</commit_message>
<xml_diff>
--- a/Week 4/exercises/results/TestCountPrimesThreadResult.xlsx
+++ b/Week 4/exercises/results/TestCountPrimesThreadResult.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianbrink/Desktop/University/Autumn 2016/PCPP/Week 4/exercises/results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-2400" windowWidth="38320" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="25605" yWindow="-2400" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="testCountPrimesThreadResult" localSheetId="0">Sheet1!$A$1:$F$33</definedName>
+    <definedName name="testCountPrimesThreadResult" localSheetId="1">Sheet1!$A$1:$F$33</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +25,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="testCountPrimesThreadResult" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="5" sourceFile="/Users/adrianbrink/Desktop/University/Autumn 2016/PCPP/Week 4/exercises/src/testCountPrimesThreadResult.txt" delimited="0">
+    <textPr fileType="mac" firstRow="5" sourceFile="/Users/adrianbrink/Desktop/University/Autumn 2016/PCPP/Week 4/exercises/src/testCountPrimesThreadResult.txt" delimited="0">
       <textFields count="7">
         <textField type="text"/>
         <textField position="21"/>
@@ -59,8 +55,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,17 +104,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -146,7 +132,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -154,32 +139,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -228,103 +192,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -360,7 +324,7 @@
                   <c:v>5236.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5111.1</c:v>
+                  <c:v>5111.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>5309.7</c:v>
@@ -375,10 +339,10 @@
                   <c:v>5097.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5214.1</c:v>
+                  <c:v>5214.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5162.0</c:v>
+                  <c:v>5162</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>5128.5</c:v>
@@ -390,7 +354,7 @@
                   <c:v>5279.1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5236.0</c:v>
+                  <c:v>5236</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>5201.8</c:v>
@@ -399,13 +363,13 @@
                   <c:v>5219.8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5224.0</c:v>
+                  <c:v>5224</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>5209.2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5186.1</c:v>
+                  <c:v>5186.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>5216.2</c:v>
@@ -437,27 +401,16 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-2095880368"/>
-        <c:axId val="-2101133328"/>
+        <c:axId val="139960704"/>
+        <c:axId val="139962624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095880368"/>
+        <c:axId val="139960704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -507,7 +460,6 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -515,29 +467,9 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -565,19 +497,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101133328"/>
+        <c:crossAx val="139962624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2101133328"/>
+        <c:axId val="139962624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -609,7 +539,6 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -617,29 +546,9 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -672,7 +581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2095880368"/>
+        <c:crossAx val="139960704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -686,7 +595,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -716,611 +624,31 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="96" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9276953" cy="6052344"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1333,7 +661,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1384,7 +712,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -1419,7 +747,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1596,31 +924,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1640,7 +968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1660,7 +988,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1680,7 +1008,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1700,7 +1028,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1720,7 +1048,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1740,7 +1068,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1760,7 +1088,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1780,7 +1108,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1800,7 +1128,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1820,7 +1148,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1840,7 +1168,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1860,7 +1188,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1880,7 +1208,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -1900,7 +1228,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1920,7 +1248,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1940,7 +1268,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1960,7 +1288,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -1980,7 +1308,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -2000,7 +1328,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2020,7 +1348,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -2040,7 +1368,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2060,7 +1388,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -2080,7 +1408,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -2100,7 +1428,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -2120,7 +1448,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -2140,7 +1468,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -2160,7 +1488,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2180,7 +1508,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -2200,7 +1528,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -2220,7 +1548,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -2240,7 +1568,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +1588,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
@@ -2283,6 +1611,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>